<commit_message>
:camera_flash: Work on bad headers
</commit_message>
<xml_diff>
--- a/tests/testthat/nourin.xlsx
+++ b/tests/testthat/nourin.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahayashi/Documents/GitHub/lucifer/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6130F8-8BD1-6E4D-BCF8-BED51C2A1352}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC33E9D8-85C3-7A46-A792-234F7ED458A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="440" windowWidth="28800" windowHeight="31960" xr2:uid="{830DF1AE-407B-458F-AD57-C80CB54B7A99}"/>
   </bookViews>
   <sheets>
-    <sheet name="matomo" sheetId="41" r:id="rId1"/>
+    <sheet name="goodheader" sheetId="41" r:id="rId1"/>
     <sheet name="北海道" sheetId="1" r:id="rId2"/>
     <sheet name="青森" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">matomo!$A:$G</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">goodheader!$A:$G</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">北海道!$A:$G</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">青森!$A:$G</definedName>
   </definedNames>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7992" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8020" uniqueCount="188">
   <si>
     <t>Ⅰ　海面漁業</t>
   </si>
@@ -678,6 +678,51 @@
   <si>
     <t>釣漁業</t>
   </si>
+  <si>
+    <t>くろまぐろ</t>
+  </si>
+  <si>
+    <t>みなみまぐろ</t>
+  </si>
+  <si>
+    <t>その他のまぐろ類</t>
+  </si>
+  <si>
+    <t>くろかじき類</t>
+  </si>
+  <si>
+    <t>その他のかじき類</t>
+  </si>
+  <si>
+    <t>そ う だかつお類</t>
+  </si>
+  <si>
+    <t>う る めい わ し</t>
+  </si>
+  <si>
+    <t>かたくちい わ し</t>
+  </si>
+  <si>
+    <t>む　　ろあ じ 類</t>
+  </si>
+  <si>
+    <t>すけとうだ　　ら</t>
+  </si>
+  <si>
+    <t>ちだい・き だ い</t>
+  </si>
+  <si>
+    <t>くろだい・へだい</t>
+  </si>
+  <si>
+    <t>おきあみ類　　　</t>
+  </si>
+  <si>
+    <t>海　　産ほ 乳 類</t>
+  </si>
+  <si>
+    <t>その他の水産動物類</t>
+  </si>
 </sst>
 </file>
 
@@ -1019,7 +1064,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1274,114 +1319,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1474,6 +1411,129 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" textRotation="255" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3921,12 +3981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3611914E-48EA-8049-B29E-C3BC198D3138}">
   <dimension ref="A1:CM45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
-      <selection pane="topRight" activeCell="H23" sqref="H23"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
-      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="CL16" sqref="CL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
@@ -4144,9 +4200,9 @@
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
-      <c r="V6" s="102"/>
-      <c r="W6" s="102"/>
-      <c r="X6" s="102"/>
+      <c r="V6" s="136"/>
+      <c r="W6" s="136"/>
+      <c r="X6" s="136"/>
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
       <c r="AA6" s="25"/>
@@ -4158,72 +4214,106 @@
       <c r="AG6" s="87"/>
       <c r="AH6" s="87"/>
       <c r="AI6" s="87"/>
-      <c r="AJ6" s="102"/>
-      <c r="AK6" s="102"/>
-      <c r="AL6" s="102"/>
-      <c r="AM6" s="102"/>
-      <c r="AN6" s="102"/>
-      <c r="AO6" s="102"/>
-      <c r="AP6" s="102"/>
-      <c r="AQ6" s="102"/>
-      <c r="AR6" s="102"/>
-      <c r="AS6" s="102"/>
-      <c r="AT6" s="102"/>
-      <c r="AU6" s="102"/>
-      <c r="AV6" s="102"/>
-      <c r="AW6" s="102"/>
-      <c r="AX6" s="102"/>
-      <c r="AY6" s="102"/>
-      <c r="AZ6" s="102"/>
-      <c r="BA6" s="102"/>
-      <c r="BB6" s="102"/>
-      <c r="BC6" s="102"/>
-      <c r="BD6" s="102"/>
-      <c r="BE6" s="102"/>
-      <c r="BF6" s="102"/>
-      <c r="BG6" s="102"/>
-      <c r="BH6" s="102"/>
-      <c r="BI6" s="102"/>
-      <c r="BJ6" s="102"/>
-      <c r="BK6" s="102"/>
+      <c r="AJ6" s="136"/>
+      <c r="AK6" s="136"/>
+      <c r="AL6" s="136"/>
+      <c r="AM6" s="136"/>
+      <c r="AN6" s="136"/>
+      <c r="AO6" s="136"/>
+      <c r="AP6" s="136"/>
+      <c r="AQ6" s="136"/>
+      <c r="AR6" s="136"/>
+      <c r="AS6" s="136"/>
+      <c r="AT6" s="136"/>
+      <c r="AU6" s="136"/>
+      <c r="AV6" s="136"/>
+      <c r="AW6" s="136"/>
+      <c r="AX6" s="136"/>
+      <c r="AY6" s="136"/>
+      <c r="AZ6" s="136"/>
+      <c r="BA6" s="136"/>
+      <c r="BB6" s="136"/>
+      <c r="BC6" s="136"/>
+      <c r="BD6" s="136"/>
+      <c r="BE6" s="136"/>
+      <c r="BF6" s="136"/>
+      <c r="BG6" s="136"/>
+      <c r="BH6" s="136"/>
+      <c r="BI6" s="136"/>
+      <c r="BJ6" s="136"/>
+      <c r="BK6" s="136"/>
       <c r="BL6" s="27"/>
-      <c r="BM6" s="88" t="s">
+      <c r="BM6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="BN6" s="89"/>
-      <c r="BO6" s="89"/>
-      <c r="BP6" s="97"/>
-      <c r="BQ6" s="98" t="s">
+      <c r="BN6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="BO6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="BP6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="BR6" s="99"/>
-      <c r="BS6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BU6" s="100"/>
+      <c r="BR6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU6" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="BV6" s="28"/>
-      <c r="BW6" s="88" t="s">
+      <c r="BW6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="BX6" s="89"/>
-      <c r="BY6" s="89"/>
-      <c r="BZ6" s="89"/>
-      <c r="CA6" s="89"/>
-      <c r="CB6" s="89"/>
-      <c r="CC6" s="29"/>
+      <c r="BX6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="BY6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="BZ6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="CA6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="CB6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC6" s="30" t="s">
+        <v>9</v>
+      </c>
       <c r="CD6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="CE6" s="23"/>
-      <c r="CF6" s="31"/>
+      <c r="CE6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF6" s="30" t="s">
+        <v>9</v>
+      </c>
       <c r="CG6" s="28"/>
       <c r="CH6" s="28"/>
       <c r="CI6" s="28"/>
       <c r="CJ6" s="28"/>
-      <c r="CK6" s="93" t="s">
+      <c r="CK6" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="CL6" s="94"/>
-      <c r="CM6" s="95"/>
+      <c r="CL6" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM6" s="156" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:91" ht="17.25" customHeight="1">
       <c r="A7" s="12"/>
@@ -4234,153 +4324,207 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="42"/>
-      <c r="I7" s="96" t="s">
+      <c r="I7" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="88" t="s">
+      <c r="J7" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="98" t="s">
+      <c r="K7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="99" t="s">
+      <c r="R7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="W7" s="99"/>
-      <c r="X7" s="100"/>
+      <c r="W7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="Y7" s="33"/>
-      <c r="Z7" s="98" t="s">
+      <c r="Z7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AA7" s="99"/>
-      <c r="AB7" s="100"/>
+      <c r="AA7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB7" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="AC7" s="34" t="s">
         <v>16</v>
       </c>
       <c r="AD7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AE7" s="101" t="s">
+      <c r="AE7" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="AF7" s="101"/>
-      <c r="AG7" s="101"/>
-      <c r="AH7" s="101"/>
-      <c r="AI7" s="101"/>
-      <c r="AJ7" s="101" t="s">
+      <c r="AF7" s="155" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG7" s="155" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH7" s="155" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI7" s="155" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ7" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="AK7" s="101"/>
-      <c r="AL7" s="101"/>
+      <c r="AK7" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL7" s="155" t="s">
+        <v>18</v>
+      </c>
       <c r="AM7" s="33" t="s">
         <v>19</v>
       </c>
       <c r="AN7" s="33"/>
       <c r="AO7" s="35"/>
-      <c r="AP7" s="98" t="s">
+      <c r="AP7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AQ7" s="99"/>
-      <c r="AR7" s="100"/>
-      <c r="AS7" s="98" t="s">
+      <c r="AQ7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="AT7" s="99"/>
-      <c r="AU7" s="100"/>
+      <c r="AT7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU7" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="AV7" s="35"/>
       <c r="AW7" s="35"/>
       <c r="AX7" s="36"/>
       <c r="AY7" s="35"/>
       <c r="AZ7" s="35"/>
       <c r="BA7" s="33"/>
-      <c r="BB7" s="88" t="s">
+      <c r="BB7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="BC7" s="89"/>
-      <c r="BD7" s="89"/>
-      <c r="BE7" s="97"/>
+      <c r="BC7" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD7" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE7" s="33" t="s">
+        <v>22</v>
+      </c>
       <c r="BF7" s="33"/>
       <c r="BG7" s="33"/>
       <c r="BH7" s="33"/>
       <c r="BI7" s="33"/>
-      <c r="BJ7" s="103" t="s">
+      <c r="BJ7" s="120" t="s">
         <v>23</v>
       </c>
       <c r="BK7" s="35"/>
-      <c r="BL7" s="90" t="s">
+      <c r="BL7" s="157" t="s">
         <v>24</v>
       </c>
       <c r="BM7" s="37"/>
       <c r="BN7" s="86"/>
-      <c r="BO7" s="90" t="s">
+      <c r="BO7" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="BP7" s="90" t="s">
+      <c r="BP7" s="122" t="s">
         <v>26</v>
       </c>
       <c r="BQ7" s="37"/>
-      <c r="BR7" s="90" t="s">
+      <c r="BR7" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="BS7" s="90" t="s">
+      <c r="BS7" s="122" t="s">
         <v>28</v>
       </c>
       <c r="BT7" s="86"/>
-      <c r="BU7" s="90" t="s">
+      <c r="BU7" s="122" t="s">
         <v>29</v>
       </c>
       <c r="BV7" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="BW7" s="96" t="s">
+        <v>185</v>
+      </c>
+      <c r="BW7" s="125" t="s">
         <v>31</v>
       </c>
       <c r="BX7" s="35"/>
       <c r="BY7" s="35"/>
       <c r="BZ7" s="35"/>
-      <c r="CA7" s="90" t="s">
+      <c r="CA7" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="CB7" s="90" t="s">
+      <c r="CB7" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="CC7" s="96" t="s">
+      <c r="CC7" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="CD7" s="90" t="s">
+      <c r="CD7" s="122" t="s">
         <v>34</v>
       </c>
       <c r="CE7" s="35"/>
-      <c r="CF7" s="90" t="s">
+      <c r="CF7" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="CG7" s="96" t="s">
+      <c r="CG7" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="CH7" s="96" t="s">
+      <c r="CH7" s="125" t="s">
         <v>37</v>
       </c>
       <c r="CI7" s="85" t="s">
-        <v>38</v>
+        <v>186</v>
       </c>
       <c r="CJ7" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="CK7" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="CK7" s="125" t="s">
         <v>31</v>
       </c>
       <c r="CL7" s="35"/>
-      <c r="CM7" s="90" t="s">
+      <c r="CM7" s="122" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4395,51 +4539,51 @@
       <c r="H8" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="96"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="37" t="s">
         <v>31</v>
       </c>
       <c r="K8" s="86" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="L8" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="M8" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="103" t="s">
+      <c r="N8" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="120" t="s">
         <v>46</v>
       </c>
       <c r="P8" s="81" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="Q8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="103" t="s">
+      <c r="R8" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="103" t="s">
+      <c r="S8" s="120" t="s">
         <v>48</v>
       </c>
       <c r="T8" s="86" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
       <c r="U8" s="81" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="V8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="103" t="s">
+      <c r="W8" s="120" t="s">
         <v>50</v>
       </c>
       <c r="X8" s="81" t="s">
-        <v>51</v>
+        <v>178</v>
       </c>
       <c r="Y8" s="85" t="s">
         <v>52</v>
@@ -4447,10 +4591,10 @@
       <c r="Z8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="AA8" s="103" t="s">
+      <c r="AA8" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="AB8" s="103" t="s">
+      <c r="AB8" s="120" t="s">
         <v>54</v>
       </c>
       <c r="AC8" s="85" t="s">
@@ -4462,26 +4606,26 @@
       <c r="AE8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="103" t="s">
+      <c r="AF8" s="120" t="s">
         <v>57</v>
       </c>
       <c r="AG8" s="86" t="s">
-        <v>58</v>
+        <v>179</v>
       </c>
       <c r="AH8" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI8" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI8" s="120" t="s">
         <v>60</v>
       </c>
       <c r="AJ8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AK8" s="103" t="s">
+      <c r="AK8" s="120" t="s">
         <v>61</v>
       </c>
       <c r="AL8" s="81" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="AM8" s="85" t="s">
         <v>63</v>
@@ -4495,20 +4639,20 @@
       <c r="AP8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AQ8" s="103" t="s">
+      <c r="AQ8" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="AR8" s="103" t="s">
+      <c r="AR8" s="120" t="s">
         <v>67</v>
       </c>
       <c r="AS8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AT8" s="103" t="s">
+      <c r="AT8" s="120" t="s">
         <v>68</v>
       </c>
       <c r="AU8" s="81" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="AV8" s="85" t="s">
         <v>70</v>
@@ -4531,14 +4675,14 @@
       <c r="BB8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="BC8" s="103" t="s">
+      <c r="BC8" s="120" t="s">
         <v>76</v>
       </c>
       <c r="BD8" s="86" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="BE8" s="81" t="s">
-        <v>78</v>
+        <v>184</v>
       </c>
       <c r="BF8" s="85" t="s">
         <v>79</v>
@@ -4552,32 +4696,30 @@
       <c r="BI8" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="BJ8" s="96"/>
+      <c r="BJ8" s="125"/>
       <c r="BK8" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="BL8" s="91"/>
+      <c r="BL8" s="158"/>
       <c r="BM8" s="37" t="s">
         <v>31</v>
       </c>
       <c r="BN8" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="BO8" s="96"/>
-      <c r="BP8" s="91"/>
+      <c r="BO8" s="125"/>
+      <c r="BP8" s="123"/>
       <c r="BQ8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="BR8" s="91"/>
-      <c r="BS8" s="91"/>
+      <c r="BR8" s="123"/>
+      <c r="BS8" s="123"/>
       <c r="BT8" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="BU8" s="91"/>
-      <c r="BV8" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="BW8" s="96"/>
+      <c r="BU8" s="123"/>
+      <c r="BV8" s="39"/>
+      <c r="BW8" s="125"/>
       <c r="BX8" s="43" t="s">
         <v>87</v>
       </c>
@@ -4587,27 +4729,23 @@
       <c r="BZ8" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="CA8" s="91"/>
-      <c r="CB8" s="91"/>
-      <c r="CC8" s="96"/>
-      <c r="CD8" s="91"/>
+      <c r="CA8" s="123"/>
+      <c r="CB8" s="123"/>
+      <c r="CC8" s="125"/>
+      <c r="CD8" s="123"/>
       <c r="CE8" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="CF8" s="91"/>
-      <c r="CG8" s="96"/>
-      <c r="CH8" s="96"/>
-      <c r="CI8" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="CJ8" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="CK8" s="96"/>
+      <c r="CF8" s="123"/>
+      <c r="CG8" s="125"/>
+      <c r="CH8" s="125"/>
+      <c r="CI8" s="85"/>
+      <c r="CJ8" s="85"/>
+      <c r="CK8" s="125"/>
       <c r="CL8" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="CM8" s="91"/>
+      <c r="CM8" s="123"/>
     </row>
     <row r="9" spans="1:91" ht="17.25" customHeight="1">
       <c r="A9" s="12"/>
@@ -4620,63 +4758,43 @@
       <c r="H9" s="82"/>
       <c r="I9" s="82"/>
       <c r="J9" s="82"/>
-      <c r="K9" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="104"/>
-      <c r="P9" s="48" t="s">
-        <v>95</v>
-      </c>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="48"/>
       <c r="Q9" s="82"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="U9" s="82" t="s">
-        <v>96</v>
-      </c>
+      <c r="R9" s="121"/>
+      <c r="S9" s="121"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="82"/>
       <c r="V9" s="46"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="82" t="s">
-        <v>97</v>
-      </c>
+      <c r="W9" s="121"/>
+      <c r="X9" s="82"/>
       <c r="Y9" s="82"/>
       <c r="Z9" s="82"/>
-      <c r="AA9" s="104"/>
-      <c r="AB9" s="104"/>
+      <c r="AA9" s="121"/>
+      <c r="AB9" s="121"/>
       <c r="AC9" s="82"/>
       <c r="AD9" s="82"/>
       <c r="AE9" s="82"/>
-      <c r="AF9" s="104"/>
-      <c r="AG9" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH9" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI9" s="104"/>
+      <c r="AF9" s="121"/>
+      <c r="AG9" s="48"/>
+      <c r="AH9" s="48"/>
+      <c r="AI9" s="121"/>
       <c r="AJ9" s="46"/>
-      <c r="AK9" s="104"/>
-      <c r="AL9" s="82" t="s">
-        <v>99</v>
-      </c>
+      <c r="AK9" s="121"/>
+      <c r="AL9" s="82"/>
       <c r="AM9" s="82"/>
       <c r="AN9" s="82"/>
       <c r="AO9" s="48"/>
       <c r="AP9" s="48"/>
-      <c r="AQ9" s="104"/>
-      <c r="AR9" s="104"/>
+      <c r="AQ9" s="121"/>
+      <c r="AR9" s="121"/>
       <c r="AS9" s="48"/>
-      <c r="AT9" s="104"/>
-      <c r="AU9" s="82" t="s">
-        <v>100</v>
-      </c>
+      <c r="AT9" s="121"/>
+      <c r="AU9" s="82"/>
       <c r="AV9" s="82"/>
       <c r="AW9" s="82"/>
       <c r="AX9" s="46"/>
@@ -4684,60 +4802,54 @@
       <c r="AZ9" s="82"/>
       <c r="BA9" s="82"/>
       <c r="BB9" s="82"/>
-      <c r="BC9" s="104"/>
-      <c r="BD9" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="BE9" s="82" t="s">
-        <v>102</v>
-      </c>
+      <c r="BC9" s="121"/>
+      <c r="BD9" s="48"/>
+      <c r="BE9" s="82"/>
       <c r="BF9" s="82"/>
       <c r="BG9" s="82"/>
       <c r="BH9" s="82"/>
       <c r="BI9" s="82"/>
-      <c r="BJ9" s="104"/>
+      <c r="BJ9" s="121"/>
       <c r="BK9" s="46"/>
-      <c r="BL9" s="92"/>
+      <c r="BL9" s="159"/>
       <c r="BM9" s="82"/>
       <c r="BN9" s="82"/>
-      <c r="BO9" s="104"/>
-      <c r="BP9" s="92"/>
+      <c r="BO9" s="121"/>
+      <c r="BP9" s="124"/>
       <c r="BQ9" s="82"/>
-      <c r="BR9" s="92"/>
-      <c r="BS9" s="92"/>
+      <c r="BR9" s="124"/>
+      <c r="BS9" s="124"/>
       <c r="BT9" s="82"/>
-      <c r="BU9" s="92"/>
+      <c r="BU9" s="124"/>
       <c r="BV9" s="82"/>
       <c r="BW9" s="82"/>
       <c r="BX9" s="46"/>
       <c r="BY9" s="82"/>
       <c r="BZ9" s="82"/>
-      <c r="CA9" s="92"/>
-      <c r="CB9" s="92"/>
+      <c r="CA9" s="124"/>
+      <c r="CB9" s="124"/>
       <c r="CC9" s="82"/>
-      <c r="CD9" s="92"/>
+      <c r="CD9" s="124"/>
       <c r="CE9" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="CF9" s="92"/>
+      <c r="CF9" s="124"/>
       <c r="CG9" s="82"/>
       <c r="CH9" s="82"/>
       <c r="CI9" s="82"/>
-      <c r="CJ9" s="82" t="s">
-        <v>86</v>
-      </c>
+      <c r="CJ9" s="82"/>
       <c r="CK9" s="82"/>
       <c r="CL9" s="82"/>
-      <c r="CM9" s="92"/>
+      <c r="CM9" s="124"/>
     </row>
     <row r="10" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
       <c r="G10" s="49">
         <v>1</v>
       </c>
@@ -4995,10 +5107,10 @@
       </c>
     </row>
     <row r="11" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="126" t="s">
+      <c r="C11" s="90" t="s">
         <v>106</v>
       </c>
       <c r="D11" s="84" t="s">
@@ -5006,7 +5118,7 @@
       </c>
       <c r="E11" s="84"/>
       <c r="F11" s="84"/>
-      <c r="G11" s="127">
+      <c r="G11" s="91">
         <v>2</v>
       </c>
       <c r="H11" s="50" t="s">
@@ -5263,10 +5375,10 @@
       </c>
     </row>
     <row r="12" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="129" t="s">
+      <c r="C12" s="93" t="s">
         <v>164</v>
       </c>
       <c r="D12" s="84" t="s">
@@ -5274,7 +5386,7 @@
       </c>
       <c r="E12" s="84"/>
       <c r="F12" s="84"/>
-      <c r="G12" s="127">
+      <c r="G12" s="91">
         <v>3</v>
       </c>
       <c r="H12" s="50" t="s">
@@ -5531,20 +5643,20 @@
       </c>
     </row>
     <row r="13" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="129" t="s">
+      <c r="C13" s="93" t="s">
         <v>164</v>
       </c>
-      <c r="D13" s="130" t="s">
+      <c r="D13" s="94" t="s">
         <v>167</v>
       </c>
-      <c r="E13" s="131" t="s">
+      <c r="E13" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="132"/>
-      <c r="G13" s="130">
+      <c r="F13" s="96"/>
+      <c r="G13" s="94">
         <v>4</v>
       </c>
       <c r="H13" s="50">
@@ -5801,20 +5913,20 @@
       </c>
     </row>
     <row r="14" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B14" s="128" t="s">
+      <c r="B14" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="129" t="s">
+      <c r="C14" s="93" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="130" t="s">
+      <c r="D14" s="94" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="133" t="s">
+      <c r="E14" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="134"/>
-      <c r="G14" s="135">
+      <c r="F14" s="98"/>
+      <c r="G14" s="99">
         <v>5</v>
       </c>
       <c r="H14" s="50" t="s">
@@ -6071,18 +6183,18 @@
       </c>
     </row>
     <row r="15" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C15" s="136" t="s">
+      <c r="C15" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="132" t="s">
+      <c r="D15" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="132"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="127">
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="91">
         <v>6</v>
       </c>
       <c r="H15" s="50">
@@ -6339,7 +6451,7 @@
       </c>
     </row>
     <row r="16" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B16" s="128" t="s">
+      <c r="B16" s="92" t="s">
         <v>162</v>
       </c>
       <c r="C16" s="83" t="s">
@@ -6348,7 +6460,7 @@
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="F16" s="84"/>
-      <c r="G16" s="127">
+      <c r="G16" s="91">
         <v>7</v>
       </c>
       <c r="H16" s="50">
@@ -6605,22 +6717,22 @@
       </c>
     </row>
     <row r="17" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B17" s="128" t="s">
+      <c r="B17" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="126" t="s">
+      <c r="C17" s="90" t="s">
         <v>118</v>
       </c>
-      <c r="D17" s="137" t="s">
+      <c r="D17" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E17" s="126" t="s">
+      <c r="E17" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="138" t="s">
+      <c r="F17" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="130">
+      <c r="G17" s="94">
         <v>8</v>
       </c>
       <c r="H17" s="50" t="s">
@@ -6877,22 +6989,22 @@
       </c>
     </row>
     <row r="18" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B18" s="128" t="s">
+      <c r="B18" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="129" t="s">
+      <c r="C18" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="137" t="s">
+      <c r="D18" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="129" t="s">
+      <c r="E18" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="F18" s="139" t="s">
+      <c r="F18" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="G18" s="140">
+      <c r="G18" s="104">
         <v>9</v>
       </c>
       <c r="H18" s="50" t="s">
@@ -7149,22 +7261,22 @@
       </c>
     </row>
     <row r="19" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="137" t="s">
+      <c r="D19" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="136" t="s">
+      <c r="E19" s="100" t="s">
         <v>171</v>
       </c>
-      <c r="F19" s="141" t="s">
+      <c r="F19" s="105" t="s">
         <v>124</v>
       </c>
-      <c r="G19" s="142">
+      <c r="G19" s="106">
         <v>10</v>
       </c>
       <c r="H19" s="50" t="s">
@@ -7421,20 +7533,20 @@
       </c>
     </row>
     <row r="20" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B20" s="128" t="s">
+      <c r="B20" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C20" s="129" t="s">
+      <c r="C20" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="137" t="s">
+      <c r="D20" s="101" t="s">
         <v>168</v>
       </c>
       <c r="E20" s="83" t="s">
         <v>125</v>
       </c>
       <c r="F20" s="84"/>
-      <c r="G20" s="127">
+      <c r="G20" s="91">
         <v>11</v>
       </c>
       <c r="H20" s="50" t="s">
@@ -7691,10 +7803,10 @@
       </c>
     </row>
     <row r="21" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C21" s="136" t="s">
+      <c r="C21" s="100" t="s">
         <v>123</v>
       </c>
       <c r="D21" s="83" t="s">
@@ -7702,7 +7814,7 @@
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="84"/>
-      <c r="G21" s="127">
+      <c r="G21" s="91">
         <v>12</v>
       </c>
       <c r="H21" s="50" t="s">
@@ -7959,18 +8071,18 @@
       </c>
     </row>
     <row r="22" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="D22" s="143" t="s">
+      <c r="D22" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="E22" s="144"/>
-      <c r="F22" s="144"/>
-      <c r="G22" s="130">
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
+      <c r="G22" s="94">
         <v>13</v>
       </c>
       <c r="H22" s="50" t="s">
@@ -8227,18 +8339,18 @@
       </c>
     </row>
     <row r="23" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="129" t="s">
+      <c r="C23" s="93" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="145" t="s">
+      <c r="D23" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="E23" s="146"/>
-      <c r="F23" s="146"/>
-      <c r="G23" s="140">
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="104">
         <v>14</v>
       </c>
       <c r="H23" s="50" t="s">
@@ -8495,18 +8607,18 @@
       </c>
     </row>
     <row r="24" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B24" s="128" t="s">
+      <c r="B24" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="136" t="s">
+      <c r="C24" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="D24" s="147" t="s">
+      <c r="D24" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="148"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="142">
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="106">
         <v>15</v>
       </c>
       <c r="H24" s="50">
@@ -8763,7 +8875,7 @@
       </c>
     </row>
     <row r="25" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B25" s="128" t="s">
+      <c r="B25" s="92" t="s">
         <v>162</v>
       </c>
       <c r="C25" s="83" t="s">
@@ -8772,7 +8884,7 @@
       <c r="D25" s="84"/>
       <c r="E25" s="84"/>
       <c r="F25" s="84"/>
-      <c r="G25" s="127">
+      <c r="G25" s="91">
         <v>16</v>
       </c>
       <c r="H25" s="50" t="s">
@@ -9029,18 +9141,18 @@
       </c>
     </row>
     <row r="26" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B26" s="128" t="s">
+      <c r="B26" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="126" t="s">
+      <c r="C26" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="131" t="s">
+      <c r="D26" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="130">
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="94">
         <v>17</v>
       </c>
       <c r="H26" s="50">
@@ -9297,18 +9409,18 @@
       </c>
     </row>
     <row r="27" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B27" s="128" t="s">
+      <c r="B27" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="129" t="s">
+      <c r="C27" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="D27" s="145" t="s">
+      <c r="D27" s="109" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="146"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="140">
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="104">
         <v>18</v>
       </c>
       <c r="H27" s="50" t="s">
@@ -9565,18 +9677,18 @@
       </c>
     </row>
     <row r="28" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B28" s="128" t="s">
+      <c r="B28" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="136" t="s">
+      <c r="C28" s="100" t="s">
         <v>166</v>
       </c>
-      <c r="D28" s="147" t="s">
+      <c r="D28" s="111" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="148"/>
-      <c r="F28" s="148"/>
-      <c r="G28" s="142">
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="106">
         <v>19</v>
       </c>
       <c r="H28" s="50">
@@ -9833,7 +9945,7 @@
       </c>
     </row>
     <row r="29" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B29" s="149" t="s">
+      <c r="B29" s="113" t="s">
         <v>162</v>
       </c>
       <c r="C29" s="83" t="s">
@@ -9842,7 +9954,7 @@
       <c r="D29" s="84"/>
       <c r="E29" s="84"/>
       <c r="F29" s="84"/>
-      <c r="G29" s="127">
+      <c r="G29" s="91">
         <v>20</v>
       </c>
       <c r="H29" s="50">
@@ -10100,20 +10212,20 @@
     </row>
     <row r="30" spans="1:91" ht="17.25" customHeight="1">
       <c r="A30" s="76"/>
-      <c r="B30" s="125" t="s">
+      <c r="B30" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="126" t="s">
+      <c r="C30" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="150" t="s">
+      <c r="D30" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="E30" s="131" t="s">
+      <c r="E30" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="F30" s="132"/>
-      <c r="G30" s="130">
+      <c r="F30" s="96"/>
+      <c r="G30" s="94">
         <v>21</v>
       </c>
       <c r="H30" s="50">
@@ -10371,20 +10483,20 @@
     </row>
     <row r="31" spans="1:91" ht="17.25" customHeight="1">
       <c r="A31" s="76"/>
-      <c r="B31" s="128" t="s">
+      <c r="B31" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="129" t="s">
+      <c r="C31" s="93" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="137" t="s">
+      <c r="D31" s="101" t="s">
         <v>169</v>
       </c>
-      <c r="E31" s="145" t="s">
+      <c r="E31" s="109" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="146"/>
-      <c r="G31" s="140">
+      <c r="F31" s="110"/>
+      <c r="G31" s="104">
         <v>22</v>
       </c>
       <c r="H31" s="50" t="s">
@@ -10642,20 +10754,20 @@
     </row>
     <row r="32" spans="1:91" ht="17.25" customHeight="1">
       <c r="A32" s="76"/>
-      <c r="B32" s="128" t="s">
+      <c r="B32" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="129" t="s">
+      <c r="C32" s="93" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="151" t="s">
+      <c r="D32" s="115" t="s">
         <v>169</v>
       </c>
-      <c r="E32" s="147" t="s">
+      <c r="E32" s="111" t="s">
         <v>143</v>
       </c>
-      <c r="F32" s="148"/>
-      <c r="G32" s="142">
+      <c r="F32" s="112"/>
+      <c r="G32" s="106">
         <v>23</v>
       </c>
       <c r="H32" s="50">
@@ -10912,18 +11024,18 @@
       </c>
     </row>
     <row r="33" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B33" s="128" t="s">
+      <c r="B33" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="D33" s="131" t="s">
+      <c r="D33" s="95" t="s">
         <v>144</v>
       </c>
       <c r="E33" s="84"/>
       <c r="F33" s="84"/>
-      <c r="G33" s="127">
+      <c r="G33" s="91">
         <v>24</v>
       </c>
       <c r="H33" s="50">
@@ -11180,20 +11292,20 @@
       </c>
     </row>
     <row r="34" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B34" s="128" t="s">
+      <c r="B34" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C34" s="126" t="s">
+      <c r="C34" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="152" t="s">
+      <c r="D34" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="131" t="s">
+      <c r="E34" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="F34" s="132"/>
-      <c r="G34" s="130">
+      <c r="F34" s="96"/>
+      <c r="G34" s="94">
         <v>25</v>
       </c>
       <c r="H34" s="50" t="s">
@@ -11450,20 +11562,20 @@
       </c>
     </row>
     <row r="35" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B35" s="128" t="s">
+      <c r="B35" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="126" t="s">
+      <c r="C35" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="137" t="s">
+      <c r="D35" s="101" t="s">
         <v>170</v>
       </c>
-      <c r="E35" s="145" t="s">
+      <c r="E35" s="109" t="s">
         <v>148</v>
       </c>
-      <c r="F35" s="146"/>
-      <c r="G35" s="140">
+      <c r="F35" s="110"/>
+      <c r="G35" s="104">
         <v>26</v>
       </c>
       <c r="H35" s="50" t="s">
@@ -11720,20 +11832,20 @@
       </c>
     </row>
     <row r="36" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B36" s="128" t="s">
+      <c r="B36" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="126" t="s">
+      <c r="C36" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="151" t="s">
+      <c r="D36" s="115" t="s">
         <v>170</v>
       </c>
-      <c r="E36" s="147" t="s">
+      <c r="E36" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="F36" s="148"/>
-      <c r="G36" s="142">
+      <c r="F36" s="112"/>
+      <c r="G36" s="106">
         <v>27</v>
       </c>
       <c r="H36" s="50" t="s">
@@ -11990,20 +12102,20 @@
       </c>
     </row>
     <row r="37" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B37" s="128" t="s">
+      <c r="B37" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C37" s="126" t="s">
+      <c r="C37" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="150" t="s">
+      <c r="D37" s="114" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="131" t="s">
+      <c r="E37" s="95" t="s">
         <v>150</v>
       </c>
-      <c r="F37" s="132"/>
-      <c r="G37" s="130">
+      <c r="F37" s="96"/>
+      <c r="G37" s="94">
         <v>28</v>
       </c>
       <c r="H37" s="50" t="s">
@@ -12260,20 +12372,20 @@
       </c>
     </row>
     <row r="38" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B38" s="128" t="s">
+      <c r="B38" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="126" t="s">
+      <c r="C38" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="137" t="s">
+      <c r="D38" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="145" t="s">
+      <c r="E38" s="109" t="s">
         <v>152</v>
       </c>
-      <c r="F38" s="146"/>
-      <c r="G38" s="140">
+      <c r="F38" s="110"/>
+      <c r="G38" s="104">
         <v>29</v>
       </c>
       <c r="H38" s="50">
@@ -12530,20 +12642,20 @@
       </c>
     </row>
     <row r="39" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B39" s="128" t="s">
+      <c r="B39" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C39" s="126" t="s">
+      <c r="C39" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="151" t="s">
+      <c r="D39" s="115" t="s">
         <v>151</v>
       </c>
-      <c r="E39" s="147" t="s">
+      <c r="E39" s="111" t="s">
         <v>153</v>
       </c>
-      <c r="F39" s="148"/>
-      <c r="G39" s="142">
+      <c r="F39" s="112"/>
+      <c r="G39" s="106">
         <v>30</v>
       </c>
       <c r="H39" s="50">
@@ -12800,18 +12912,18 @@
       </c>
     </row>
     <row r="40" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B40" s="128" t="s">
+      <c r="B40" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="C40" s="126" t="s">
+      <c r="C40" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="131" t="s">
+      <c r="D40" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="E40" s="132"/>
-      <c r="F40" s="132"/>
-      <c r="G40" s="130">
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="94">
         <v>31</v>
       </c>
       <c r="H40" s="50">
@@ -13068,18 +13180,18 @@
       </c>
     </row>
     <row r="41" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B41" s="149" t="s">
+      <c r="B41" s="113" t="s">
         <v>172</v>
       </c>
-      <c r="C41" s="126" t="s">
+      <c r="C41" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="D41" s="133" t="s">
+      <c r="D41" s="97" t="s">
         <v>155</v>
       </c>
-      <c r="E41" s="134"/>
-      <c r="F41" s="134"/>
-      <c r="G41" s="135">
+      <c r="E41" s="98"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="99">
         <v>32</v>
       </c>
       <c r="H41" s="50">
@@ -13345,7 +13457,7 @@
       <c r="D42" s="84"/>
       <c r="E42" s="84"/>
       <c r="F42" s="84"/>
-      <c r="G42" s="127">
+      <c r="G42" s="91">
         <v>33</v>
       </c>
       <c r="H42" s="50" t="s">
@@ -13602,16 +13714,16 @@
       </c>
     </row>
     <row r="43" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B43" s="132" t="s">
+      <c r="B43" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="C43" s="124" t="s">
+      <c r="C43" s="88" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="130">
+      <c r="D43" s="88"/>
+      <c r="E43" s="88"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="94">
         <v>34</v>
       </c>
       <c r="H43" s="50">
@@ -13868,16 +13980,16 @@
       </c>
     </row>
     <row r="44" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B44" s="148" t="s">
+      <c r="B44" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="153" t="s">
+      <c r="C44" s="117" t="s">
         <v>160</v>
       </c>
-      <c r="D44" s="154"/>
-      <c r="E44" s="154"/>
-      <c r="F44" s="154"/>
-      <c r="G44" s="135">
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="99">
         <v>35</v>
       </c>
       <c r="H44" s="79">
@@ -14143,12 +14255,23 @@
     </row>
   </sheetData>
   <dataConsolidate link="1"/>
-  <mergeCells count="52">
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="AI8:AI9"/>
-    <mergeCell ref="AK8:AK9"/>
-    <mergeCell ref="AQ8:AQ9"/>
+  <mergeCells count="37">
+    <mergeCell ref="BP7:BP9"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="AJ6:AW6"/>
+    <mergeCell ref="AX6:BK6"/>
+    <mergeCell ref="BJ7:BJ9"/>
+    <mergeCell ref="BO7:BO9"/>
+    <mergeCell ref="CG7:CG8"/>
+    <mergeCell ref="CH7:CH8"/>
+    <mergeCell ref="CK7:CK8"/>
+    <mergeCell ref="BR7:BR9"/>
+    <mergeCell ref="BS7:BS9"/>
+    <mergeCell ref="BU7:BU9"/>
+    <mergeCell ref="BW7:BW8"/>
+    <mergeCell ref="CA7:CA9"/>
+    <mergeCell ref="CB7:CB9"/>
     <mergeCell ref="AR8:AR9"/>
     <mergeCell ref="AT8:AT9"/>
     <mergeCell ref="BC8:BC9"/>
@@ -14165,37 +14288,11 @@
     <mergeCell ref="CC7:CC8"/>
     <mergeCell ref="CD7:CD9"/>
     <mergeCell ref="CF7:CF9"/>
-    <mergeCell ref="CG7:CG8"/>
-    <mergeCell ref="CH7:CH8"/>
-    <mergeCell ref="CK7:CK8"/>
-    <mergeCell ref="BR7:BR9"/>
-    <mergeCell ref="BS7:BS9"/>
-    <mergeCell ref="BU7:BU9"/>
-    <mergeCell ref="BW7:BW8"/>
-    <mergeCell ref="CA7:CA9"/>
-    <mergeCell ref="CB7:CB9"/>
-    <mergeCell ref="AS7:AU7"/>
-    <mergeCell ref="BB7:BE7"/>
-    <mergeCell ref="BJ7:BJ9"/>
-    <mergeCell ref="BL7:BL9"/>
-    <mergeCell ref="BO7:BO9"/>
-    <mergeCell ref="BP7:BP9"/>
-    <mergeCell ref="BZ6:CB6"/>
-    <mergeCell ref="CK6:CM6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Z7:AB7"/>
-    <mergeCell ref="AE7:AI7"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="AJ6:AW6"/>
-    <mergeCell ref="AX6:BK6"/>
-    <mergeCell ref="BM6:BP6"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="BW6:BY6"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="AI8:AI9"/>
+    <mergeCell ref="AK8:AK9"/>
+    <mergeCell ref="AQ8:AQ9"/>
   </mergeCells>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.51181102362204722" right="0.19685039370078741" top="0.31496062992125984" bottom="0.27559055118110237" header="0.39370078740157483" footer="0.27559055118110237"/>
@@ -14220,7 +14317,7 @@
       <selection activeCell="H23" sqref="H23"/>
       <selection pane="topRight" activeCell="H23" sqref="H23"/>
       <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31:B40"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
@@ -14443,9 +14540,9 @@
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
-      <c r="V6" s="102"/>
-      <c r="W6" s="102"/>
-      <c r="X6" s="102"/>
+      <c r="V6" s="136"/>
+      <c r="W6" s="136"/>
+      <c r="X6" s="136"/>
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
       <c r="AA6" s="25"/>
@@ -14457,57 +14554,57 @@
       <c r="AG6" s="26"/>
       <c r="AH6" s="26"/>
       <c r="AI6" s="26"/>
-      <c r="AJ6" s="102"/>
-      <c r="AK6" s="102"/>
-      <c r="AL6" s="102"/>
-      <c r="AM6" s="102"/>
-      <c r="AN6" s="102"/>
-      <c r="AO6" s="102"/>
-      <c r="AP6" s="102"/>
-      <c r="AQ6" s="102"/>
-      <c r="AR6" s="102"/>
-      <c r="AS6" s="102"/>
-      <c r="AT6" s="102"/>
-      <c r="AU6" s="102"/>
-      <c r="AV6" s="102"/>
-      <c r="AW6" s="102"/>
-      <c r="AX6" s="102"/>
-      <c r="AY6" s="102"/>
-      <c r="AZ6" s="102"/>
-      <c r="BA6" s="102"/>
-      <c r="BB6" s="102"/>
-      <c r="BC6" s="102"/>
-      <c r="BD6" s="102"/>
-      <c r="BE6" s="102"/>
-      <c r="BF6" s="102"/>
-      <c r="BG6" s="102"/>
-      <c r="BH6" s="102"/>
-      <c r="BI6" s="102"/>
-      <c r="BJ6" s="102"/>
-      <c r="BK6" s="102"/>
+      <c r="AJ6" s="136"/>
+      <c r="AK6" s="136"/>
+      <c r="AL6" s="136"/>
+      <c r="AM6" s="136"/>
+      <c r="AN6" s="136"/>
+      <c r="AO6" s="136"/>
+      <c r="AP6" s="136"/>
+      <c r="AQ6" s="136"/>
+      <c r="AR6" s="136"/>
+      <c r="AS6" s="136"/>
+      <c r="AT6" s="136"/>
+      <c r="AU6" s="136"/>
+      <c r="AV6" s="136"/>
+      <c r="AW6" s="136"/>
+      <c r="AX6" s="136"/>
+      <c r="AY6" s="136"/>
+      <c r="AZ6" s="136"/>
+      <c r="BA6" s="136"/>
+      <c r="BB6" s="136"/>
+      <c r="BC6" s="136"/>
+      <c r="BD6" s="136"/>
+      <c r="BE6" s="136"/>
+      <c r="BF6" s="136"/>
+      <c r="BG6" s="136"/>
+      <c r="BH6" s="136"/>
+      <c r="BI6" s="136"/>
+      <c r="BJ6" s="136"/>
+      <c r="BK6" s="136"/>
       <c r="BL6" s="27"/>
-      <c r="BM6" s="88" t="s">
+      <c r="BM6" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="BN6" s="89"/>
-      <c r="BO6" s="89"/>
-      <c r="BP6" s="97"/>
-      <c r="BQ6" s="98" t="s">
+      <c r="BN6" s="130"/>
+      <c r="BO6" s="130"/>
+      <c r="BP6" s="131"/>
+      <c r="BQ6" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="BR6" s="99"/>
-      <c r="BS6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BU6" s="100"/>
+      <c r="BR6" s="127"/>
+      <c r="BS6" s="127"/>
+      <c r="BT6" s="127"/>
+      <c r="BU6" s="128"/>
       <c r="BV6" s="28"/>
-      <c r="BW6" s="88" t="s">
+      <c r="BW6" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="BX6" s="89"/>
-      <c r="BY6" s="89"/>
-      <c r="BZ6" s="89"/>
-      <c r="CA6" s="89"/>
-      <c r="CB6" s="89"/>
+      <c r="BX6" s="130"/>
+      <c r="BY6" s="130"/>
+      <c r="BZ6" s="130"/>
+      <c r="CA6" s="130"/>
+      <c r="CB6" s="130"/>
       <c r="CC6" s="29"/>
       <c r="CD6" s="30" t="s">
         <v>9</v>
@@ -14518,11 +14615,11 @@
       <c r="CH6" s="28"/>
       <c r="CI6" s="28"/>
       <c r="CJ6" s="28"/>
-      <c r="CK6" s="93" t="s">
+      <c r="CK6" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="CL6" s="94"/>
-      <c r="CM6" s="95"/>
+      <c r="CL6" s="133"/>
+      <c r="CM6" s="134"/>
     </row>
     <row r="7" spans="1:91" ht="17.25" customHeight="1">
       <c r="A7" s="12"/>
@@ -14533,140 +14630,140 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="32"/>
-      <c r="I7" s="96" t="s">
+      <c r="I7" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="88" t="s">
+      <c r="J7" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="98" t="s">
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="99" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="127"/>
+      <c r="T7" s="127"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="W7" s="99"/>
-      <c r="X7" s="100"/>
+      <c r="W7" s="127"/>
+      <c r="X7" s="128"/>
       <c r="Y7" s="33"/>
-      <c r="Z7" s="98" t="s">
+      <c r="Z7" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="AA7" s="99"/>
-      <c r="AB7" s="100"/>
+      <c r="AA7" s="127"/>
+      <c r="AB7" s="128"/>
       <c r="AC7" s="34" t="s">
         <v>16</v>
       </c>
       <c r="AD7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AE7" s="101" t="s">
+      <c r="AE7" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="AF7" s="101"/>
-      <c r="AG7" s="101"/>
-      <c r="AH7" s="101"/>
-      <c r="AI7" s="101"/>
-      <c r="AJ7" s="101" t="s">
+      <c r="AF7" s="135"/>
+      <c r="AG7" s="135"/>
+      <c r="AH7" s="135"/>
+      <c r="AI7" s="135"/>
+      <c r="AJ7" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="AK7" s="101"/>
-      <c r="AL7" s="101"/>
+      <c r="AK7" s="135"/>
+      <c r="AL7" s="135"/>
       <c r="AM7" s="33" t="s">
         <v>19</v>
       </c>
       <c r="AN7" s="33"/>
       <c r="AO7" s="35"/>
-      <c r="AP7" s="98" t="s">
+      <c r="AP7" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="AQ7" s="99"/>
-      <c r="AR7" s="100"/>
-      <c r="AS7" s="98" t="s">
+      <c r="AQ7" s="127"/>
+      <c r="AR7" s="128"/>
+      <c r="AS7" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="AT7" s="99"/>
-      <c r="AU7" s="100"/>
+      <c r="AT7" s="127"/>
+      <c r="AU7" s="128"/>
       <c r="AV7" s="35"/>
       <c r="AW7" s="35"/>
       <c r="AX7" s="36"/>
       <c r="AY7" s="35"/>
       <c r="AZ7" s="35"/>
       <c r="BA7" s="33"/>
-      <c r="BB7" s="88" t="s">
+      <c r="BB7" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="BC7" s="89"/>
-      <c r="BD7" s="89"/>
-      <c r="BE7" s="97"/>
+      <c r="BC7" s="130"/>
+      <c r="BD7" s="130"/>
+      <c r="BE7" s="131"/>
       <c r="BF7" s="33"/>
       <c r="BG7" s="33"/>
       <c r="BH7" s="33"/>
       <c r="BI7" s="33"/>
-      <c r="BJ7" s="103" t="s">
+      <c r="BJ7" s="120" t="s">
         <v>23</v>
       </c>
       <c r="BK7" s="35"/>
-      <c r="BL7" s="90" t="s">
+      <c r="BL7" s="122" t="s">
         <v>24</v>
       </c>
       <c r="BM7" s="37"/>
       <c r="BN7" s="38"/>
-      <c r="BO7" s="90" t="s">
+      <c r="BO7" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="BP7" s="90" t="s">
+      <c r="BP7" s="122" t="s">
         <v>26</v>
       </c>
       <c r="BQ7" s="37"/>
-      <c r="BR7" s="90" t="s">
+      <c r="BR7" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="BS7" s="90" t="s">
+      <c r="BS7" s="122" t="s">
         <v>28</v>
       </c>
       <c r="BT7" s="38"/>
-      <c r="BU7" s="90" t="s">
+      <c r="BU7" s="122" t="s">
         <v>29</v>
       </c>
       <c r="BV7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="BW7" s="96" t="s">
+      <c r="BW7" s="125" t="s">
         <v>31</v>
       </c>
       <c r="BX7" s="35"/>
       <c r="BY7" s="35"/>
       <c r="BZ7" s="35"/>
-      <c r="CA7" s="90" t="s">
+      <c r="CA7" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="CB7" s="90" t="s">
+      <c r="CB7" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="CC7" s="96" t="s">
+      <c r="CC7" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="CD7" s="90" t="s">
+      <c r="CD7" s="122" t="s">
         <v>34</v>
       </c>
       <c r="CE7" s="35"/>
-      <c r="CF7" s="90" t="s">
+      <c r="CF7" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="CG7" s="96" t="s">
+      <c r="CG7" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="CH7" s="96" t="s">
+      <c r="CH7" s="125" t="s">
         <v>37</v>
       </c>
       <c r="CI7" s="40" t="s">
@@ -14675,11 +14772,11 @@
       <c r="CJ7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="CK7" s="96" t="s">
+      <c r="CK7" s="125" t="s">
         <v>31</v>
       </c>
       <c r="CL7" s="35"/>
-      <c r="CM7" s="90" t="s">
+      <c r="CM7" s="122" t="s">
         <v>40</v>
       </c>
     </row>
@@ -14694,7 +14791,7 @@
       <c r="H8" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="96"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="37" t="s">
         <v>31</v>
       </c>
@@ -14704,13 +14801,13 @@
       <c r="L8" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="103" t="s">
+      <c r="M8" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="103" t="s">
+      <c r="N8" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="120" t="s">
         <v>46</v>
       </c>
       <c r="P8" s="41" t="s">
@@ -14719,10 +14816,10 @@
       <c r="Q8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="103" t="s">
+      <c r="R8" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="103" t="s">
+      <c r="S8" s="120" t="s">
         <v>48</v>
       </c>
       <c r="T8" s="38" t="s">
@@ -14734,7 +14831,7 @@
       <c r="V8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="103" t="s">
+      <c r="W8" s="120" t="s">
         <v>50</v>
       </c>
       <c r="X8" s="41" t="s">
@@ -14746,10 +14843,10 @@
       <c r="Z8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="AA8" s="103" t="s">
+      <c r="AA8" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="AB8" s="103" t="s">
+      <c r="AB8" s="120" t="s">
         <v>54</v>
       </c>
       <c r="AC8" s="40" t="s">
@@ -14761,7 +14858,7 @@
       <c r="AE8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="103" t="s">
+      <c r="AF8" s="120" t="s">
         <v>57</v>
       </c>
       <c r="AG8" s="38" t="s">
@@ -14770,13 +14867,13 @@
       <c r="AH8" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="AI8" s="103" t="s">
+      <c r="AI8" s="120" t="s">
         <v>60</v>
       </c>
       <c r="AJ8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AK8" s="103" t="s">
+      <c r="AK8" s="120" t="s">
         <v>61</v>
       </c>
       <c r="AL8" s="41" t="s">
@@ -14794,16 +14891,16 @@
       <c r="AP8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AQ8" s="103" t="s">
+      <c r="AQ8" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="AR8" s="103" t="s">
+      <c r="AR8" s="120" t="s">
         <v>67</v>
       </c>
       <c r="AS8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AT8" s="103" t="s">
+      <c r="AT8" s="120" t="s">
         <v>68</v>
       </c>
       <c r="AU8" s="41" t="s">
@@ -14830,7 +14927,7 @@
       <c r="BB8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="BC8" s="103" t="s">
+      <c r="BC8" s="120" t="s">
         <v>76</v>
       </c>
       <c r="BD8" s="38" t="s">
@@ -14851,32 +14948,32 @@
       <c r="BI8" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="BJ8" s="96"/>
+      <c r="BJ8" s="125"/>
       <c r="BK8" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="BL8" s="91"/>
+      <c r="BL8" s="123"/>
       <c r="BM8" s="37" t="s">
         <v>31</v>
       </c>
       <c r="BN8" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="BO8" s="96"/>
-      <c r="BP8" s="91"/>
+      <c r="BO8" s="125"/>
+      <c r="BP8" s="123"/>
       <c r="BQ8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="BR8" s="91"/>
-      <c r="BS8" s="91"/>
+      <c r="BR8" s="123"/>
+      <c r="BS8" s="123"/>
       <c r="BT8" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="BU8" s="91"/>
+      <c r="BU8" s="123"/>
       <c r="BV8" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="BW8" s="96"/>
+      <c r="BW8" s="125"/>
       <c r="BX8" s="43" t="s">
         <v>87</v>
       </c>
@@ -14886,27 +14983,27 @@
       <c r="BZ8" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="CA8" s="91"/>
-      <c r="CB8" s="91"/>
-      <c r="CC8" s="96"/>
-      <c r="CD8" s="91"/>
+      <c r="CA8" s="123"/>
+      <c r="CB8" s="123"/>
+      <c r="CC8" s="125"/>
+      <c r="CD8" s="123"/>
       <c r="CE8" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="CF8" s="91"/>
-      <c r="CG8" s="96"/>
-      <c r="CH8" s="96"/>
+      <c r="CF8" s="123"/>
+      <c r="CG8" s="125"/>
+      <c r="CH8" s="125"/>
       <c r="CI8" s="40" t="s">
         <v>91</v>
       </c>
       <c r="CJ8" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="CK8" s="96"/>
+      <c r="CK8" s="125"/>
       <c r="CL8" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="CM8" s="91"/>
+      <c r="CM8" s="123"/>
     </row>
     <row r="9" spans="1:91" ht="17.25" customHeight="1">
       <c r="A9" s="12"/>
@@ -14925,15 +15022,15 @@
       <c r="L9" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="104"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
       <c r="P9" s="48" t="s">
         <v>95</v>
       </c>
       <c r="Q9" s="47"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="121"/>
       <c r="T9" s="48" t="s">
         <v>96</v>
       </c>
@@ -14941,27 +15038,27 @@
         <v>96</v>
       </c>
       <c r="V9" s="46"/>
-      <c r="W9" s="104"/>
+      <c r="W9" s="121"/>
       <c r="X9" s="47" t="s">
         <v>97</v>
       </c>
       <c r="Y9" s="47"/>
       <c r="Z9" s="47"/>
-      <c r="AA9" s="104"/>
-      <c r="AB9" s="104"/>
+      <c r="AA9" s="121"/>
+      <c r="AB9" s="121"/>
       <c r="AC9" s="47"/>
       <c r="AD9" s="47"/>
       <c r="AE9" s="47"/>
-      <c r="AF9" s="104"/>
+      <c r="AF9" s="121"/>
       <c r="AG9" s="48" t="s">
         <v>98</v>
       </c>
       <c r="AH9" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="AI9" s="104"/>
+      <c r="AI9" s="121"/>
       <c r="AJ9" s="46"/>
-      <c r="AK9" s="104"/>
+      <c r="AK9" s="121"/>
       <c r="AL9" s="47" t="s">
         <v>99</v>
       </c>
@@ -14969,10 +15066,10 @@
       <c r="AN9" s="47"/>
       <c r="AO9" s="48"/>
       <c r="AP9" s="48"/>
-      <c r="AQ9" s="104"/>
-      <c r="AR9" s="104"/>
+      <c r="AQ9" s="121"/>
+      <c r="AR9" s="121"/>
       <c r="AS9" s="48"/>
-      <c r="AT9" s="104"/>
+      <c r="AT9" s="121"/>
       <c r="AU9" s="47" t="s">
         <v>100</v>
       </c>
@@ -14983,7 +15080,7 @@
       <c r="AZ9" s="47"/>
       <c r="BA9" s="47"/>
       <c r="BB9" s="47"/>
-      <c r="BC9" s="104"/>
+      <c r="BC9" s="121"/>
       <c r="BD9" s="48" t="s">
         <v>101</v>
       </c>
@@ -14994,31 +15091,31 @@
       <c r="BG9" s="47"/>
       <c r="BH9" s="47"/>
       <c r="BI9" s="47"/>
-      <c r="BJ9" s="104"/>
+      <c r="BJ9" s="121"/>
       <c r="BK9" s="46"/>
-      <c r="BL9" s="92"/>
+      <c r="BL9" s="124"/>
       <c r="BM9" s="47"/>
       <c r="BN9" s="47"/>
-      <c r="BO9" s="104"/>
-      <c r="BP9" s="92"/>
+      <c r="BO9" s="121"/>
+      <c r="BP9" s="124"/>
       <c r="BQ9" s="47"/>
-      <c r="BR9" s="92"/>
-      <c r="BS9" s="92"/>
+      <c r="BR9" s="124"/>
+      <c r="BS9" s="124"/>
       <c r="BT9" s="47"/>
-      <c r="BU9" s="92"/>
+      <c r="BU9" s="124"/>
       <c r="BV9" s="47"/>
       <c r="BW9" s="47"/>
       <c r="BX9" s="46"/>
       <c r="BY9" s="47"/>
       <c r="BZ9" s="47"/>
-      <c r="CA9" s="92"/>
-      <c r="CB9" s="92"/>
+      <c r="CA9" s="124"/>
+      <c r="CB9" s="124"/>
       <c r="CC9" s="47"/>
-      <c r="CD9" s="92"/>
+      <c r="CD9" s="124"/>
       <c r="CE9" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="CF9" s="92"/>
+      <c r="CF9" s="124"/>
       <c r="CG9" s="47"/>
       <c r="CH9" s="47"/>
       <c r="CI9" s="47"/>
@@ -15027,16 +15124,16 @@
       </c>
       <c r="CK9" s="47"/>
       <c r="CL9" s="47"/>
-      <c r="CM9" s="92"/>
+      <c r="CM9" s="124"/>
     </row>
     <row r="10" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
       <c r="G10" s="49">
         <v>1</v>
       </c>
@@ -15295,7 +15392,7 @@
     </row>
     <row r="11" spans="1:91" ht="17.25" customHeight="1">
       <c r="B11" s="51"/>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="141" t="s">
         <v>106</v>
       </c>
       <c r="D11" s="52" t="s">
@@ -15560,10 +15657,10 @@
       </c>
     </row>
     <row r="12" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="144" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="110"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="52" t="s">
         <v>110</v>
       </c>
@@ -15826,8 +15923,8 @@
       </c>
     </row>
     <row r="13" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B13" s="123"/>
-      <c r="C13" s="110"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="142"/>
       <c r="D13" s="54" t="s">
         <v>112</v>
       </c>
@@ -16092,8 +16189,8 @@
       </c>
     </row>
     <row r="14" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B14" s="123"/>
-      <c r="C14" s="110"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="142"/>
       <c r="D14" s="58" t="s">
         <v>114</v>
       </c>
@@ -16358,8 +16455,8 @@
       </c>
     </row>
     <row r="15" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B15" s="123"/>
-      <c r="C15" s="111"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="143"/>
       <c r="D15" s="56" t="s">
         <v>116</v>
       </c>
@@ -16622,13 +16719,13 @@
       </c>
     </row>
     <row r="16" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B16" s="123"/>
-      <c r="C16" s="113" t="s">
+      <c r="B16" s="144"/>
+      <c r="C16" s="150" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
       <c r="G16" s="53">
         <v>7</v>
       </c>
@@ -16886,12 +16983,12 @@
       </c>
     </row>
     <row r="17" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B17" s="123"/>
-      <c r="C17" s="109" t="s">
+      <c r="B17" s="144"/>
+      <c r="C17" s="141" t="s">
         <v>118</v>
       </c>
       <c r="D17" s="62"/>
-      <c r="E17" s="109" t="s">
+      <c r="E17" s="141" t="s">
         <v>119</v>
       </c>
       <c r="F17" s="63" t="s">
@@ -17154,12 +17251,12 @@
       </c>
     </row>
     <row r="18" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B18" s="123"/>
-      <c r="C18" s="110"/>
+      <c r="B18" s="144"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="110"/>
+      <c r="E18" s="142"/>
       <c r="F18" s="64" t="s">
         <v>122</v>
       </c>
@@ -17420,12 +17517,12 @@
       </c>
     </row>
     <row r="19" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B19" s="123"/>
-      <c r="C19" s="110"/>
+      <c r="B19" s="144"/>
+      <c r="C19" s="142"/>
       <c r="D19" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="111"/>
+      <c r="E19" s="143"/>
       <c r="F19" s="66" t="s">
         <v>124</v>
       </c>
@@ -17686,13 +17783,13 @@
       </c>
     </row>
     <row r="20" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B20" s="123"/>
-      <c r="C20" s="110"/>
+      <c r="B20" s="144"/>
+      <c r="C20" s="142"/>
       <c r="D20" s="62"/>
-      <c r="E20" s="115" t="s">
+      <c r="E20" s="152" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="116"/>
+      <c r="F20" s="153"/>
       <c r="G20" s="53">
         <v>11</v>
       </c>
@@ -17950,13 +18047,13 @@
       </c>
     </row>
     <row r="21" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B21" s="123"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="113" t="s">
+      <c r="B21" s="144"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
       <c r="G21" s="53">
         <v>12</v>
       </c>
@@ -18214,8 +18311,8 @@
       </c>
     </row>
     <row r="22" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B22" s="123"/>
-      <c r="C22" s="109" t="s">
+      <c r="B22" s="144"/>
+      <c r="C22" s="141" t="s">
         <v>127</v>
       </c>
       <c r="D22" s="68" t="s">
@@ -18480,8 +18577,8 @@
       </c>
     </row>
     <row r="23" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B23" s="123"/>
-      <c r="C23" s="110"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="142"/>
       <c r="D23" s="70" t="s">
         <v>129</v>
       </c>
@@ -18744,8 +18841,8 @@
       </c>
     </row>
     <row r="24" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B24" s="123"/>
-      <c r="C24" s="111"/>
+      <c r="B24" s="144"/>
+      <c r="C24" s="143"/>
       <c r="D24" s="72" t="s">
         <v>130</v>
       </c>
@@ -19008,13 +19105,13 @@
       </c>
     </row>
     <row r="25" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B25" s="123"/>
-      <c r="C25" s="113" t="s">
+      <c r="B25" s="144"/>
+      <c r="C25" s="150" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
+      <c r="D25" s="151"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
       <c r="G25" s="53">
         <v>16</v>
       </c>
@@ -19272,8 +19369,8 @@
       </c>
     </row>
     <row r="26" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B26" s="123"/>
-      <c r="C26" s="109" t="s">
+      <c r="B26" s="144"/>
+      <c r="C26" s="141" t="s">
         <v>132</v>
       </c>
       <c r="D26" s="55" t="s">
@@ -19538,8 +19635,8 @@
       </c>
     </row>
     <row r="27" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B27" s="123"/>
-      <c r="C27" s="110"/>
+      <c r="B27" s="144"/>
+      <c r="C27" s="142"/>
       <c r="D27" s="70" t="s">
         <v>134</v>
       </c>
@@ -19802,8 +19899,8 @@
       </c>
     </row>
     <row r="28" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B28" s="123"/>
-      <c r="C28" s="111"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="143"/>
       <c r="D28" s="72" t="s">
         <v>135</v>
       </c>
@@ -20332,7 +20429,7 @@
     <row r="30" spans="1:91" ht="17.25" customHeight="1">
       <c r="A30" s="76"/>
       <c r="B30" s="57"/>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="141" t="s">
         <v>137</v>
       </c>
       <c r="D30" s="77" t="s">
@@ -20600,10 +20697,10 @@
     </row>
     <row r="31" spans="1:91" ht="17.25" customHeight="1">
       <c r="A31" s="76"/>
-      <c r="B31" s="123" t="s">
+      <c r="B31" s="144" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="110"/>
+      <c r="C31" s="142"/>
       <c r="D31" s="62"/>
       <c r="E31" s="70" t="s">
         <v>141</v>
@@ -20867,8 +20964,8 @@
     </row>
     <row r="32" spans="1:91" ht="17.25" customHeight="1">
       <c r="A32" s="76"/>
-      <c r="B32" s="123"/>
-      <c r="C32" s="110"/>
+      <c r="B32" s="144"/>
+      <c r="C32" s="142"/>
       <c r="D32" s="78" t="s">
         <v>142</v>
       </c>
@@ -21133,8 +21230,8 @@
       </c>
     </row>
     <row r="33" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B33" s="123"/>
-      <c r="C33" s="111"/>
+      <c r="B33" s="144"/>
+      <c r="C33" s="143"/>
       <c r="D33" s="55" t="s">
         <v>144</v>
       </c>
@@ -21397,11 +21494,11 @@
       </c>
     </row>
     <row r="34" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B34" s="123"/>
-      <c r="C34" s="109" t="s">
+      <c r="B34" s="144"/>
+      <c r="C34" s="141" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="105" t="s">
+      <c r="D34" s="147" t="s">
         <v>146</v>
       </c>
       <c r="E34" s="55" t="s">
@@ -21665,9 +21762,9 @@
       </c>
     </row>
     <row r="35" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B35" s="123"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="106"/>
+      <c r="B35" s="144"/>
+      <c r="C35" s="142"/>
+      <c r="D35" s="148"/>
       <c r="E35" s="70" t="s">
         <v>148</v>
       </c>
@@ -21929,9 +22026,9 @@
       </c>
     </row>
     <row r="36" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B36" s="123"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="107"/>
+      <c r="B36" s="144"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="149"/>
       <c r="E36" s="72" t="s">
         <v>149</v>
       </c>
@@ -22193,8 +22290,8 @@
       </c>
     </row>
     <row r="37" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B37" s="123"/>
-      <c r="C37" s="110"/>
+      <c r="B37" s="144"/>
+      <c r="C37" s="142"/>
       <c r="D37" s="77"/>
       <c r="E37" s="55" t="s">
         <v>150</v>
@@ -22457,8 +22554,8 @@
       </c>
     </row>
     <row r="38" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B38" s="123"/>
-      <c r="C38" s="110"/>
+      <c r="B38" s="144"/>
+      <c r="C38" s="142"/>
       <c r="D38" s="62" t="s">
         <v>151</v>
       </c>
@@ -22723,8 +22820,8 @@
       </c>
     </row>
     <row r="39" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B39" s="123"/>
-      <c r="C39" s="110"/>
+      <c r="B39" s="144"/>
+      <c r="C39" s="142"/>
       <c r="D39" s="78"/>
       <c r="E39" s="72" t="s">
         <v>153</v>
@@ -22987,8 +23084,8 @@
       </c>
     </row>
     <row r="40" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B40" s="123"/>
-      <c r="C40" s="110"/>
+      <c r="B40" s="144"/>
+      <c r="C40" s="142"/>
       <c r="D40" s="55" t="s">
         <v>154</v>
       </c>
@@ -23252,7 +23349,7 @@
     </row>
     <row r="41" spans="2:91" ht="17.25" customHeight="1">
       <c r="B41" s="67"/>
-      <c r="C41" s="111"/>
+      <c r="C41" s="143"/>
       <c r="D41" s="59" t="s">
         <v>155</v>
       </c>
@@ -23515,10 +23612,10 @@
       </c>
     </row>
     <row r="42" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="145" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="122"/>
+      <c r="C42" s="146"/>
       <c r="D42" s="75" t="s">
         <v>157</v>
       </c>
@@ -23781,10 +23878,10 @@
       </c>
     </row>
     <row r="43" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B43" s="117" t="s">
+      <c r="B43" s="137" t="s">
         <v>158</v>
       </c>
-      <c r="C43" s="118"/>
+      <c r="C43" s="138"/>
       <c r="D43" s="56" t="s">
         <v>159</v>
       </c>
@@ -24047,8 +24144,8 @@
       </c>
     </row>
     <row r="44" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B44" s="119"/>
-      <c r="C44" s="120"/>
+      <c r="B44" s="139"/>
+      <c r="C44" s="140"/>
       <c r="D44" s="59" t="s">
         <v>160</v>
       </c>
@@ -24321,27 +24418,36 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="67">
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="AK8:AK9"/>
-    <mergeCell ref="AQ8:AQ9"/>
-    <mergeCell ref="AR8:AR9"/>
-    <mergeCell ref="AT8:AT9"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="B12:B28"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="BW6:BY6"/>
+    <mergeCell ref="BP7:BP9"/>
+    <mergeCell ref="BZ6:CB6"/>
+    <mergeCell ref="CK6:CM6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="AE7:AI7"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="AJ6:AW6"/>
+    <mergeCell ref="AX6:BK6"/>
+    <mergeCell ref="BM6:BP6"/>
+    <mergeCell ref="BQ6:BU6"/>
+    <mergeCell ref="AS7:AU7"/>
+    <mergeCell ref="BB7:BE7"/>
+    <mergeCell ref="BJ7:BJ9"/>
+    <mergeCell ref="BL7:BL9"/>
+    <mergeCell ref="BO7:BO9"/>
+    <mergeCell ref="BC8:BC9"/>
+    <mergeCell ref="CK7:CK8"/>
+    <mergeCell ref="BR7:BR9"/>
+    <mergeCell ref="BS7:BS9"/>
+    <mergeCell ref="BU7:BU9"/>
+    <mergeCell ref="BW7:BW8"/>
+    <mergeCell ref="CA7:CA9"/>
+    <mergeCell ref="CB7:CB9"/>
     <mergeCell ref="CM7:CM9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
@@ -24358,36 +24464,27 @@
     <mergeCell ref="CG7:CG8"/>
     <mergeCell ref="CH7:CH8"/>
     <mergeCell ref="AI8:AI9"/>
-    <mergeCell ref="CK7:CK8"/>
-    <mergeCell ref="BR7:BR9"/>
-    <mergeCell ref="BS7:BS9"/>
-    <mergeCell ref="BU7:BU9"/>
-    <mergeCell ref="BW7:BW8"/>
-    <mergeCell ref="CA7:CA9"/>
-    <mergeCell ref="CB7:CB9"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="AS7:AU7"/>
-    <mergeCell ref="BB7:BE7"/>
-    <mergeCell ref="BJ7:BJ9"/>
-    <mergeCell ref="BL7:BL9"/>
-    <mergeCell ref="BO7:BO9"/>
-    <mergeCell ref="BC8:BC9"/>
-    <mergeCell ref="BW6:BY6"/>
-    <mergeCell ref="BP7:BP9"/>
-    <mergeCell ref="BZ6:CB6"/>
-    <mergeCell ref="CK6:CM6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Z7:AB7"/>
-    <mergeCell ref="AE7:AI7"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="AJ6:AW6"/>
-    <mergeCell ref="AX6:BK6"/>
-    <mergeCell ref="BM6:BP6"/>
+    <mergeCell ref="AK8:AK9"/>
+    <mergeCell ref="AQ8:AQ9"/>
+    <mergeCell ref="AR8:AR9"/>
+    <mergeCell ref="AT8:AT9"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B12:B28"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions gridLines="1" gridLinesSet="0"/>
@@ -24636,9 +24733,9 @@
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
-      <c r="V6" s="102"/>
-      <c r="W6" s="102"/>
-      <c r="X6" s="102"/>
+      <c r="V6" s="136"/>
+      <c r="W6" s="136"/>
+      <c r="X6" s="136"/>
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
       <c r="AA6" s="25"/>
@@ -24650,57 +24747,57 @@
       <c r="AG6" s="26"/>
       <c r="AH6" s="26"/>
       <c r="AI6" s="26"/>
-      <c r="AJ6" s="102"/>
-      <c r="AK6" s="102"/>
-      <c r="AL6" s="102"/>
-      <c r="AM6" s="102"/>
-      <c r="AN6" s="102"/>
-      <c r="AO6" s="102"/>
-      <c r="AP6" s="102"/>
-      <c r="AQ6" s="102"/>
-      <c r="AR6" s="102"/>
-      <c r="AS6" s="102"/>
-      <c r="AT6" s="102"/>
-      <c r="AU6" s="102"/>
-      <c r="AV6" s="102"/>
-      <c r="AW6" s="102"/>
-      <c r="AX6" s="102"/>
-      <c r="AY6" s="102"/>
-      <c r="AZ6" s="102"/>
-      <c r="BA6" s="102"/>
-      <c r="BB6" s="102"/>
-      <c r="BC6" s="102"/>
-      <c r="BD6" s="102"/>
-      <c r="BE6" s="102"/>
-      <c r="BF6" s="102"/>
-      <c r="BG6" s="102"/>
-      <c r="BH6" s="102"/>
-      <c r="BI6" s="102"/>
-      <c r="BJ6" s="102"/>
-      <c r="BK6" s="102"/>
+      <c r="AJ6" s="136"/>
+      <c r="AK6" s="136"/>
+      <c r="AL6" s="136"/>
+      <c r="AM6" s="136"/>
+      <c r="AN6" s="136"/>
+      <c r="AO6" s="136"/>
+      <c r="AP6" s="136"/>
+      <c r="AQ6" s="136"/>
+      <c r="AR6" s="136"/>
+      <c r="AS6" s="136"/>
+      <c r="AT6" s="136"/>
+      <c r="AU6" s="136"/>
+      <c r="AV6" s="136"/>
+      <c r="AW6" s="136"/>
+      <c r="AX6" s="136"/>
+      <c r="AY6" s="136"/>
+      <c r="AZ6" s="136"/>
+      <c r="BA6" s="136"/>
+      <c r="BB6" s="136"/>
+      <c r="BC6" s="136"/>
+      <c r="BD6" s="136"/>
+      <c r="BE6" s="136"/>
+      <c r="BF6" s="136"/>
+      <c r="BG6" s="136"/>
+      <c r="BH6" s="136"/>
+      <c r="BI6" s="136"/>
+      <c r="BJ6" s="136"/>
+      <c r="BK6" s="136"/>
       <c r="BL6" s="27"/>
-      <c r="BM6" s="88" t="s">
+      <c r="BM6" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="BN6" s="89"/>
-      <c r="BO6" s="89"/>
-      <c r="BP6" s="97"/>
-      <c r="BQ6" s="98" t="s">
+      <c r="BN6" s="130"/>
+      <c r="BO6" s="130"/>
+      <c r="BP6" s="131"/>
+      <c r="BQ6" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="BR6" s="99"/>
-      <c r="BS6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BU6" s="100"/>
+      <c r="BR6" s="127"/>
+      <c r="BS6" s="127"/>
+      <c r="BT6" s="127"/>
+      <c r="BU6" s="128"/>
       <c r="BV6" s="28"/>
-      <c r="BW6" s="88" t="s">
+      <c r="BW6" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="BX6" s="89"/>
-      <c r="BY6" s="89"/>
-      <c r="BZ6" s="89"/>
-      <c r="CA6" s="89"/>
-      <c r="CB6" s="89"/>
+      <c r="BX6" s="130"/>
+      <c r="BY6" s="130"/>
+      <c r="BZ6" s="130"/>
+      <c r="CA6" s="130"/>
+      <c r="CB6" s="130"/>
       <c r="CC6" s="29"/>
       <c r="CD6" s="30" t="s">
         <v>9</v>
@@ -24711,11 +24808,11 @@
       <c r="CH6" s="28"/>
       <c r="CI6" s="28"/>
       <c r="CJ6" s="28"/>
-      <c r="CK6" s="93" t="s">
+      <c r="CK6" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="CL6" s="94"/>
-      <c r="CM6" s="95"/>
+      <c r="CL6" s="133"/>
+      <c r="CM6" s="134"/>
     </row>
     <row r="7" spans="1:91" ht="17.25" customHeight="1">
       <c r="A7" s="12"/>
@@ -24726,140 +24823,140 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="42"/>
-      <c r="I7" s="96" t="s">
+      <c r="I7" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="88" t="s">
+      <c r="J7" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="98" t="s">
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="99" t="s">
+      <c r="R7" s="127"/>
+      <c r="S7" s="127"/>
+      <c r="T7" s="127"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="W7" s="99"/>
-      <c r="X7" s="100"/>
+      <c r="W7" s="127"/>
+      <c r="X7" s="128"/>
       <c r="Y7" s="33"/>
-      <c r="Z7" s="98" t="s">
+      <c r="Z7" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="AA7" s="99"/>
-      <c r="AB7" s="100"/>
+      <c r="AA7" s="127"/>
+      <c r="AB7" s="128"/>
       <c r="AC7" s="34" t="s">
         <v>16</v>
       </c>
       <c r="AD7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AE7" s="101" t="s">
+      <c r="AE7" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="AF7" s="101"/>
-      <c r="AG7" s="101"/>
-      <c r="AH7" s="101"/>
-      <c r="AI7" s="101"/>
-      <c r="AJ7" s="101" t="s">
+      <c r="AF7" s="135"/>
+      <c r="AG7" s="135"/>
+      <c r="AH7" s="135"/>
+      <c r="AI7" s="135"/>
+      <c r="AJ7" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="AK7" s="101"/>
-      <c r="AL7" s="101"/>
+      <c r="AK7" s="135"/>
+      <c r="AL7" s="135"/>
       <c r="AM7" s="33" t="s">
         <v>19</v>
       </c>
       <c r="AN7" s="33"/>
       <c r="AO7" s="35"/>
-      <c r="AP7" s="98" t="s">
+      <c r="AP7" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="AQ7" s="99"/>
-      <c r="AR7" s="100"/>
-      <c r="AS7" s="98" t="s">
+      <c r="AQ7" s="127"/>
+      <c r="AR7" s="128"/>
+      <c r="AS7" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="AT7" s="99"/>
-      <c r="AU7" s="100"/>
+      <c r="AT7" s="127"/>
+      <c r="AU7" s="128"/>
       <c r="AV7" s="35"/>
       <c r="AW7" s="35"/>
       <c r="AX7" s="36"/>
       <c r="AY7" s="35"/>
       <c r="AZ7" s="35"/>
       <c r="BA7" s="33"/>
-      <c r="BB7" s="88" t="s">
+      <c r="BB7" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="BC7" s="89"/>
-      <c r="BD7" s="89"/>
-      <c r="BE7" s="97"/>
+      <c r="BC7" s="130"/>
+      <c r="BD7" s="130"/>
+      <c r="BE7" s="131"/>
       <c r="BF7" s="33"/>
       <c r="BG7" s="33"/>
       <c r="BH7" s="33"/>
       <c r="BI7" s="33"/>
-      <c r="BJ7" s="103" t="s">
+      <c r="BJ7" s="120" t="s">
         <v>23</v>
       </c>
       <c r="BK7" s="35"/>
-      <c r="BL7" s="90" t="s">
+      <c r="BL7" s="122" t="s">
         <v>24</v>
       </c>
       <c r="BM7" s="37"/>
       <c r="BN7" s="38"/>
-      <c r="BO7" s="90" t="s">
+      <c r="BO7" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="BP7" s="90" t="s">
+      <c r="BP7" s="122" t="s">
         <v>26</v>
       </c>
       <c r="BQ7" s="37"/>
-      <c r="BR7" s="90" t="s">
+      <c r="BR7" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="BS7" s="90" t="s">
+      <c r="BS7" s="122" t="s">
         <v>28</v>
       </c>
       <c r="BT7" s="38"/>
-      <c r="BU7" s="90" t="s">
+      <c r="BU7" s="122" t="s">
         <v>29</v>
       </c>
       <c r="BV7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="BW7" s="96" t="s">
+      <c r="BW7" s="125" t="s">
         <v>31</v>
       </c>
       <c r="BX7" s="35"/>
       <c r="BY7" s="35"/>
       <c r="BZ7" s="35"/>
-      <c r="CA7" s="90" t="s">
+      <c r="CA7" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="CB7" s="90" t="s">
+      <c r="CB7" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="CC7" s="96" t="s">
+      <c r="CC7" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="CD7" s="90" t="s">
+      <c r="CD7" s="122" t="s">
         <v>34</v>
       </c>
       <c r="CE7" s="35"/>
-      <c r="CF7" s="90" t="s">
+      <c r="CF7" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="CG7" s="96" t="s">
+      <c r="CG7" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="CH7" s="96" t="s">
+      <c r="CH7" s="125" t="s">
         <v>37</v>
       </c>
       <c r="CI7" s="40" t="s">
@@ -24868,11 +24965,11 @@
       <c r="CJ7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="CK7" s="96" t="s">
+      <c r="CK7" s="125" t="s">
         <v>31</v>
       </c>
       <c r="CL7" s="35"/>
-      <c r="CM7" s="90" t="s">
+      <c r="CM7" s="122" t="s">
         <v>40</v>
       </c>
     </row>
@@ -24887,7 +24984,7 @@
       <c r="H8" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="96"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="37" t="s">
         <v>31</v>
       </c>
@@ -24897,13 +24994,13 @@
       <c r="L8" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="103" t="s">
+      <c r="M8" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="103" t="s">
+      <c r="N8" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="120" t="s">
         <v>46</v>
       </c>
       <c r="P8" s="41" t="s">
@@ -24912,10 +25009,10 @@
       <c r="Q8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="103" t="s">
+      <c r="R8" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="103" t="s">
+      <c r="S8" s="120" t="s">
         <v>48</v>
       </c>
       <c r="T8" s="38" t="s">
@@ -24927,7 +25024,7 @@
       <c r="V8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="103" t="s">
+      <c r="W8" s="120" t="s">
         <v>50</v>
       </c>
       <c r="X8" s="41" t="s">
@@ -24939,10 +25036,10 @@
       <c r="Z8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="AA8" s="103" t="s">
+      <c r="AA8" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="AB8" s="103" t="s">
+      <c r="AB8" s="120" t="s">
         <v>54</v>
       </c>
       <c r="AC8" s="40" t="s">
@@ -24954,7 +25051,7 @@
       <c r="AE8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="103" t="s">
+      <c r="AF8" s="120" t="s">
         <v>57</v>
       </c>
       <c r="AG8" s="38" t="s">
@@ -24963,13 +25060,13 @@
       <c r="AH8" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="AI8" s="103" t="s">
+      <c r="AI8" s="120" t="s">
         <v>60</v>
       </c>
       <c r="AJ8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AK8" s="103" t="s">
+      <c r="AK8" s="120" t="s">
         <v>61</v>
       </c>
       <c r="AL8" s="41" t="s">
@@ -24987,16 +25084,16 @@
       <c r="AP8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AQ8" s="103" t="s">
+      <c r="AQ8" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="AR8" s="103" t="s">
+      <c r="AR8" s="120" t="s">
         <v>67</v>
       </c>
       <c r="AS8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AT8" s="103" t="s">
+      <c r="AT8" s="120" t="s">
         <v>68</v>
       </c>
       <c r="AU8" s="41" t="s">
@@ -25023,7 +25120,7 @@
       <c r="BB8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="BC8" s="103" t="s">
+      <c r="BC8" s="120" t="s">
         <v>76</v>
       </c>
       <c r="BD8" s="38" t="s">
@@ -25044,32 +25141,32 @@
       <c r="BI8" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="BJ8" s="96"/>
+      <c r="BJ8" s="125"/>
       <c r="BK8" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="BL8" s="91"/>
+      <c r="BL8" s="123"/>
       <c r="BM8" s="37" t="s">
         <v>31</v>
       </c>
       <c r="BN8" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="BO8" s="96"/>
-      <c r="BP8" s="91"/>
+      <c r="BO8" s="125"/>
+      <c r="BP8" s="123"/>
       <c r="BQ8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="BR8" s="91"/>
-      <c r="BS8" s="91"/>
+      <c r="BR8" s="123"/>
+      <c r="BS8" s="123"/>
       <c r="BT8" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="BU8" s="91"/>
+      <c r="BU8" s="123"/>
       <c r="BV8" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="BW8" s="96"/>
+      <c r="BW8" s="125"/>
       <c r="BX8" s="43" t="s">
         <v>87</v>
       </c>
@@ -25079,27 +25176,27 @@
       <c r="BZ8" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="CA8" s="91"/>
-      <c r="CB8" s="91"/>
-      <c r="CC8" s="96"/>
-      <c r="CD8" s="91"/>
+      <c r="CA8" s="123"/>
+      <c r="CB8" s="123"/>
+      <c r="CC8" s="125"/>
+      <c r="CD8" s="123"/>
       <c r="CE8" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="CF8" s="91"/>
-      <c r="CG8" s="96"/>
-      <c r="CH8" s="96"/>
+      <c r="CF8" s="123"/>
+      <c r="CG8" s="125"/>
+      <c r="CH8" s="125"/>
       <c r="CI8" s="40" t="s">
         <v>91</v>
       </c>
       <c r="CJ8" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="CK8" s="96"/>
+      <c r="CK8" s="125"/>
       <c r="CL8" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="CM8" s="91"/>
+      <c r="CM8" s="123"/>
     </row>
     <row r="9" spans="1:91" ht="17.25" customHeight="1">
       <c r="A9" s="12"/>
@@ -25118,15 +25215,15 @@
       <c r="L9" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="104"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
       <c r="P9" s="48" t="s">
         <v>95</v>
       </c>
       <c r="Q9" s="47"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="121"/>
       <c r="T9" s="48" t="s">
         <v>96</v>
       </c>
@@ -25134,27 +25231,27 @@
         <v>96</v>
       </c>
       <c r="V9" s="46"/>
-      <c r="W9" s="104"/>
+      <c r="W9" s="121"/>
       <c r="X9" s="47" t="s">
         <v>97</v>
       </c>
       <c r="Y9" s="47"/>
       <c r="Z9" s="47"/>
-      <c r="AA9" s="104"/>
-      <c r="AB9" s="104"/>
+      <c r="AA9" s="121"/>
+      <c r="AB9" s="121"/>
       <c r="AC9" s="47"/>
       <c r="AD9" s="47"/>
       <c r="AE9" s="47"/>
-      <c r="AF9" s="104"/>
+      <c r="AF9" s="121"/>
       <c r="AG9" s="48" t="s">
         <v>98</v>
       </c>
       <c r="AH9" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="AI9" s="104"/>
+      <c r="AI9" s="121"/>
       <c r="AJ9" s="46"/>
-      <c r="AK9" s="104"/>
+      <c r="AK9" s="121"/>
       <c r="AL9" s="47" t="s">
         <v>99</v>
       </c>
@@ -25162,10 +25259,10 @@
       <c r="AN9" s="47"/>
       <c r="AO9" s="48"/>
       <c r="AP9" s="48"/>
-      <c r="AQ9" s="104"/>
-      <c r="AR9" s="104"/>
+      <c r="AQ9" s="121"/>
+      <c r="AR9" s="121"/>
       <c r="AS9" s="48"/>
-      <c r="AT9" s="104"/>
+      <c r="AT9" s="121"/>
       <c r="AU9" s="47" t="s">
         <v>100</v>
       </c>
@@ -25176,7 +25273,7 @@
       <c r="AZ9" s="47"/>
       <c r="BA9" s="47"/>
       <c r="BB9" s="47"/>
-      <c r="BC9" s="104"/>
+      <c r="BC9" s="121"/>
       <c r="BD9" s="48" t="s">
         <v>101</v>
       </c>
@@ -25187,31 +25284,31 @@
       <c r="BG9" s="47"/>
       <c r="BH9" s="47"/>
       <c r="BI9" s="47"/>
-      <c r="BJ9" s="104"/>
+      <c r="BJ9" s="121"/>
       <c r="BK9" s="46"/>
-      <c r="BL9" s="92"/>
+      <c r="BL9" s="124"/>
       <c r="BM9" s="47"/>
       <c r="BN9" s="47"/>
-      <c r="BO9" s="104"/>
-      <c r="BP9" s="92"/>
+      <c r="BO9" s="121"/>
+      <c r="BP9" s="124"/>
       <c r="BQ9" s="47"/>
-      <c r="BR9" s="92"/>
-      <c r="BS9" s="92"/>
+      <c r="BR9" s="124"/>
+      <c r="BS9" s="124"/>
       <c r="BT9" s="47"/>
-      <c r="BU9" s="92"/>
+      <c r="BU9" s="124"/>
       <c r="BV9" s="47"/>
       <c r="BW9" s="47"/>
       <c r="BX9" s="46"/>
       <c r="BY9" s="47"/>
       <c r="BZ9" s="47"/>
-      <c r="CA9" s="92"/>
-      <c r="CB9" s="92"/>
+      <c r="CA9" s="124"/>
+      <c r="CB9" s="124"/>
       <c r="CC9" s="47"/>
-      <c r="CD9" s="92"/>
+      <c r="CD9" s="124"/>
       <c r="CE9" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="CF9" s="92"/>
+      <c r="CF9" s="124"/>
       <c r="CG9" s="47"/>
       <c r="CH9" s="47"/>
       <c r="CI9" s="47"/>
@@ -25220,16 +25317,16 @@
       </c>
       <c r="CK9" s="47"/>
       <c r="CL9" s="47"/>
-      <c r="CM9" s="92"/>
+      <c r="CM9" s="124"/>
     </row>
     <row r="10" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
       <c r="G10" s="49">
         <v>1</v>
       </c>
@@ -25488,7 +25585,7 @@
     </row>
     <row r="11" spans="1:91" ht="17.25" customHeight="1">
       <c r="B11" s="51"/>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="141" t="s">
         <v>106</v>
       </c>
       <c r="D11" s="52" t="s">
@@ -25753,10 +25850,10 @@
       </c>
     </row>
     <row r="12" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="110"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="52" t="s">
         <v>110</v>
       </c>
@@ -26019,8 +26116,8 @@
       </c>
     </row>
     <row r="13" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B13" s="112"/>
-      <c r="C13" s="110"/>
+      <c r="B13" s="154"/>
+      <c r="C13" s="142"/>
       <c r="D13" s="54" t="s">
         <v>112</v>
       </c>
@@ -26285,8 +26382,8 @@
       </c>
     </row>
     <row r="14" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B14" s="112"/>
-      <c r="C14" s="110"/>
+      <c r="B14" s="154"/>
+      <c r="C14" s="142"/>
       <c r="D14" s="58" t="s">
         <v>114</v>
       </c>
@@ -26551,8 +26648,8 @@
       </c>
     </row>
     <row r="15" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B15" s="112"/>
-      <c r="C15" s="111"/>
+      <c r="B15" s="154"/>
+      <c r="C15" s="143"/>
       <c r="D15" s="56" t="s">
         <v>116</v>
       </c>
@@ -26815,13 +26912,13 @@
       </c>
     </row>
     <row r="16" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B16" s="112"/>
-      <c r="C16" s="113" t="s">
+      <c r="B16" s="154"/>
+      <c r="C16" s="150" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
       <c r="G16" s="53">
         <v>7</v>
       </c>
@@ -27079,12 +27176,12 @@
       </c>
     </row>
     <row r="17" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B17" s="112"/>
-      <c r="C17" s="109" t="s">
+      <c r="B17" s="154"/>
+      <c r="C17" s="141" t="s">
         <v>118</v>
       </c>
       <c r="D17" s="62"/>
-      <c r="E17" s="109" t="s">
+      <c r="E17" s="141" t="s">
         <v>119</v>
       </c>
       <c r="F17" s="63" t="s">
@@ -27347,12 +27444,12 @@
       </c>
     </row>
     <row r="18" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B18" s="112"/>
-      <c r="C18" s="110"/>
+      <c r="B18" s="154"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="110"/>
+      <c r="E18" s="142"/>
       <c r="F18" s="64" t="s">
         <v>122</v>
       </c>
@@ -27613,12 +27710,12 @@
       </c>
     </row>
     <row r="19" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B19" s="112"/>
-      <c r="C19" s="110"/>
+      <c r="B19" s="154"/>
+      <c r="C19" s="142"/>
       <c r="D19" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="111"/>
+      <c r="E19" s="143"/>
       <c r="F19" s="66" t="s">
         <v>124</v>
       </c>
@@ -27879,13 +27976,13 @@
       </c>
     </row>
     <row r="20" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B20" s="112"/>
-      <c r="C20" s="110"/>
+      <c r="B20" s="154"/>
+      <c r="C20" s="142"/>
       <c r="D20" s="62"/>
-      <c r="E20" s="115" t="s">
+      <c r="E20" s="152" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="116"/>
+      <c r="F20" s="153"/>
       <c r="G20" s="53">
         <v>11</v>
       </c>
@@ -28143,13 +28240,13 @@
       </c>
     </row>
     <row r="21" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B21" s="112"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="113" t="s">
+      <c r="B21" s="154"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
       <c r="G21" s="53">
         <v>12</v>
       </c>
@@ -28407,8 +28504,8 @@
       </c>
     </row>
     <row r="22" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B22" s="112"/>
-      <c r="C22" s="109" t="s">
+      <c r="B22" s="154"/>
+      <c r="C22" s="141" t="s">
         <v>127</v>
       </c>
       <c r="D22" s="68" t="s">
@@ -28673,8 +28770,8 @@
       </c>
     </row>
     <row r="23" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B23" s="112"/>
-      <c r="C23" s="110"/>
+      <c r="B23" s="154"/>
+      <c r="C23" s="142"/>
       <c r="D23" s="70" t="s">
         <v>129</v>
       </c>
@@ -28937,8 +29034,8 @@
       </c>
     </row>
     <row r="24" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B24" s="112"/>
-      <c r="C24" s="111"/>
+      <c r="B24" s="154"/>
+      <c r="C24" s="143"/>
       <c r="D24" s="72" t="s">
         <v>130</v>
       </c>
@@ -29201,13 +29298,13 @@
       </c>
     </row>
     <row r="25" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B25" s="112"/>
-      <c r="C25" s="113" t="s">
+      <c r="B25" s="154"/>
+      <c r="C25" s="150" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
+      <c r="D25" s="151"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
       <c r="G25" s="53">
         <v>16</v>
       </c>
@@ -29465,8 +29562,8 @@
       </c>
     </row>
     <row r="26" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B26" s="112"/>
-      <c r="C26" s="109" t="s">
+      <c r="B26" s="154"/>
+      <c r="C26" s="141" t="s">
         <v>132</v>
       </c>
       <c r="D26" s="55" t="s">
@@ -29731,8 +29828,8 @@
       </c>
     </row>
     <row r="27" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B27" s="112"/>
-      <c r="C27" s="110"/>
+      <c r="B27" s="154"/>
+      <c r="C27" s="142"/>
       <c r="D27" s="70" t="s">
         <v>134</v>
       </c>
@@ -29995,8 +30092,8 @@
       </c>
     </row>
     <row r="28" spans="1:91" ht="17.25" customHeight="1">
-      <c r="B28" s="112"/>
-      <c r="C28" s="111"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="143"/>
       <c r="D28" s="72" t="s">
         <v>135</v>
       </c>
@@ -30525,7 +30622,7 @@
     <row r="30" spans="1:91" ht="17.25" customHeight="1">
       <c r="A30" s="76"/>
       <c r="B30" s="57"/>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="141" t="s">
         <v>137</v>
       </c>
       <c r="D30" s="77" t="s">
@@ -30793,10 +30890,10 @@
     </row>
     <row r="31" spans="1:91" ht="17.25" customHeight="1">
       <c r="A31" s="76"/>
-      <c r="B31" s="112" t="s">
+      <c r="B31" s="154" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="110"/>
+      <c r="C31" s="142"/>
       <c r="D31" s="62"/>
       <c r="E31" s="70" t="s">
         <v>141</v>
@@ -31060,8 +31157,8 @@
     </row>
     <row r="32" spans="1:91" ht="17.25" customHeight="1">
       <c r="A32" s="76"/>
-      <c r="B32" s="112"/>
-      <c r="C32" s="110"/>
+      <c r="B32" s="154"/>
+      <c r="C32" s="142"/>
       <c r="D32" s="78" t="s">
         <v>142</v>
       </c>
@@ -31326,8 +31423,8 @@
       </c>
     </row>
     <row r="33" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B33" s="112"/>
-      <c r="C33" s="111"/>
+      <c r="B33" s="154"/>
+      <c r="C33" s="143"/>
       <c r="D33" s="55" t="s">
         <v>144</v>
       </c>
@@ -31590,11 +31687,11 @@
       </c>
     </row>
     <row r="34" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B34" s="112"/>
-      <c r="C34" s="109" t="s">
+      <c r="B34" s="154"/>
+      <c r="C34" s="141" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="105" t="s">
+      <c r="D34" s="147" t="s">
         <v>146</v>
       </c>
       <c r="E34" s="55" t="s">
@@ -31858,9 +31955,9 @@
       </c>
     </row>
     <row r="35" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B35" s="112"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="106"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="142"/>
+      <c r="D35" s="148"/>
       <c r="E35" s="70" t="s">
         <v>148</v>
       </c>
@@ -32122,9 +32219,9 @@
       </c>
     </row>
     <row r="36" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B36" s="112"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="107"/>
+      <c r="B36" s="154"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="149"/>
       <c r="E36" s="72" t="s">
         <v>149</v>
       </c>
@@ -32386,8 +32483,8 @@
       </c>
     </row>
     <row r="37" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B37" s="112"/>
-      <c r="C37" s="110"/>
+      <c r="B37" s="154"/>
+      <c r="C37" s="142"/>
       <c r="D37" s="77"/>
       <c r="E37" s="55" t="s">
         <v>150</v>
@@ -32650,8 +32747,8 @@
       </c>
     </row>
     <row r="38" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B38" s="112"/>
-      <c r="C38" s="110"/>
+      <c r="B38" s="154"/>
+      <c r="C38" s="142"/>
       <c r="D38" s="62" t="s">
         <v>151</v>
       </c>
@@ -32916,8 +33013,8 @@
       </c>
     </row>
     <row r="39" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B39" s="112"/>
-      <c r="C39" s="110"/>
+      <c r="B39" s="154"/>
+      <c r="C39" s="142"/>
       <c r="D39" s="78"/>
       <c r="E39" s="72" t="s">
         <v>153</v>
@@ -33180,8 +33277,8 @@
       </c>
     </row>
     <row r="40" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B40" s="112"/>
-      <c r="C40" s="110"/>
+      <c r="B40" s="154"/>
+      <c r="C40" s="142"/>
       <c r="D40" s="55" t="s">
         <v>154</v>
       </c>
@@ -33445,7 +33542,7 @@
     </row>
     <row r="41" spans="2:91" ht="17.25" customHeight="1">
       <c r="B41" s="67"/>
-      <c r="C41" s="111"/>
+      <c r="C41" s="143"/>
       <c r="D41" s="59" t="s">
         <v>155</v>
       </c>
@@ -33708,10 +33805,10 @@
       </c>
     </row>
     <row r="42" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="145" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="122"/>
+      <c r="C42" s="146"/>
       <c r="D42" s="75" t="s">
         <v>157</v>
       </c>
@@ -33974,10 +34071,10 @@
       </c>
     </row>
     <row r="43" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B43" s="117" t="s">
+      <c r="B43" s="137" t="s">
         <v>158</v>
       </c>
-      <c r="C43" s="118"/>
+      <c r="C43" s="138"/>
       <c r="D43" s="56" t="s">
         <v>159</v>
       </c>
@@ -34240,8 +34337,8 @@
       </c>
     </row>
     <row r="44" spans="2:91" ht="17.25" customHeight="1">
-      <c r="B44" s="119"/>
-      <c r="C44" s="120"/>
+      <c r="B44" s="139"/>
+      <c r="C44" s="140"/>
       <c r="D44" s="59" t="s">
         <v>160</v>
       </c>
@@ -34514,27 +34611,36 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="67">
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="AK8:AK9"/>
-    <mergeCell ref="AQ8:AQ9"/>
-    <mergeCell ref="AR8:AR9"/>
-    <mergeCell ref="AT8:AT9"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="B12:B28"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="BW6:BY6"/>
+    <mergeCell ref="BP7:BP9"/>
+    <mergeCell ref="BZ6:CB6"/>
+    <mergeCell ref="CK6:CM6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="AE7:AI7"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="AJ6:AW6"/>
+    <mergeCell ref="AX6:BK6"/>
+    <mergeCell ref="BM6:BP6"/>
+    <mergeCell ref="BQ6:BU6"/>
+    <mergeCell ref="AS7:AU7"/>
+    <mergeCell ref="BB7:BE7"/>
+    <mergeCell ref="BJ7:BJ9"/>
+    <mergeCell ref="BL7:BL9"/>
+    <mergeCell ref="BO7:BO9"/>
+    <mergeCell ref="BC8:BC9"/>
+    <mergeCell ref="CK7:CK8"/>
+    <mergeCell ref="BR7:BR9"/>
+    <mergeCell ref="BS7:BS9"/>
+    <mergeCell ref="BU7:BU9"/>
+    <mergeCell ref="BW7:BW8"/>
+    <mergeCell ref="CA7:CA9"/>
+    <mergeCell ref="CB7:CB9"/>
     <mergeCell ref="CM7:CM9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
@@ -34551,36 +34657,27 @@
     <mergeCell ref="CG7:CG8"/>
     <mergeCell ref="CH7:CH8"/>
     <mergeCell ref="AI8:AI9"/>
-    <mergeCell ref="CK7:CK8"/>
-    <mergeCell ref="BR7:BR9"/>
-    <mergeCell ref="BS7:BS9"/>
-    <mergeCell ref="BU7:BU9"/>
-    <mergeCell ref="BW7:BW8"/>
-    <mergeCell ref="CA7:CA9"/>
-    <mergeCell ref="CB7:CB9"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="AS7:AU7"/>
-    <mergeCell ref="BB7:BE7"/>
-    <mergeCell ref="BJ7:BJ9"/>
-    <mergeCell ref="BL7:BL9"/>
-    <mergeCell ref="BO7:BO9"/>
-    <mergeCell ref="BC8:BC9"/>
-    <mergeCell ref="BW6:BY6"/>
-    <mergeCell ref="BP7:BP9"/>
-    <mergeCell ref="BZ6:CB6"/>
-    <mergeCell ref="CK6:CM6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Z7:AB7"/>
-    <mergeCell ref="AE7:AI7"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="AJ6:AW6"/>
-    <mergeCell ref="AX6:BK6"/>
-    <mergeCell ref="BM6:BP6"/>
+    <mergeCell ref="AK8:AK9"/>
+    <mergeCell ref="AQ8:AQ9"/>
+    <mergeCell ref="AR8:AR9"/>
+    <mergeCell ref="AT8:AT9"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B12:B28"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions gridLines="1" gridLinesSet="0"/>

</xml_diff>